<commit_message>
before good idea split task
</commit_message>
<xml_diff>
--- a/ipynb/module_prgem/sizes_ruby_sap_sto.xlsx
+++ b/ipynb/module_prgem/sizes_ruby_sap_sto.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -139,7 +139,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -147,9 +147,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +187,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -257,7 +257,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -431,159 +431,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+      <c r="D4">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D6">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D7">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D8">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>0.1</v>
-      </c>
-      <c r="E3">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
-        <v>0.25</v>
-      </c>
-      <c r="E4">
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>75</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>0.5</v>
-      </c>
-      <c r="E5">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>100</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1.99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>125</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
-        <v>150</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>3.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1">
-        <v>175</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
       <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
         <v>4.99</v>
       </c>
     </row>

</xml_diff>